<commit_message>
add PB1-1 and PB1-2
</commit_message>
<xml_diff>
--- a/configurations.xlsx
+++ b/configurations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,20 +20,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Notes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>red is input parameter, black font is calculated parameter, yellow highlights changed parameters</t>
+    </r>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>PB1-1</t>
+  </si>
+  <si>
+    <t>PB1-2</t>
+  </si>
+  <si>
+    <t>PB1-3</t>
+  </si>
+  <si>
+    <t>perigee x apogee (miles)</t>
+  </si>
+  <si>
+    <t>88.8 x 90.2</t>
+  </si>
+  <si>
+    <t>200.6 x 205.5</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>engine mass comparison</t>
+  </si>
+  <si>
     <t>created</t>
   </si>
   <si>
     <t>simulated</t>
   </si>
   <si>
-    <t>performance</t>
-  </si>
-  <si>
     <t>Common</t>
   </si>
   <si>
@@ -61,9 +102,6 @@
     <t>oxi capacity</t>
   </si>
   <si>
-    <t>lbm</t>
-  </si>
-  <si>
     <t>fuel capacity</t>
   </si>
   <si>
@@ -83,9 +121,6 @@
   </si>
   <si>
     <t>propellant load</t>
-  </si>
-  <si>
-    <t>fraction</t>
   </si>
   <si>
     <t>nozzle diameter</t>
@@ -128,11 +163,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -164,12 +200,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,7 +257,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,7 +273,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,308 +366,439 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>42459</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>42459</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>75</v>
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>42459</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>42459</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>3</v>
+      <c r="A9" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>96.46</v>
+        <v>75</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>13.78</v>
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>230</v>
+        <v>43.75</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>43.75</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>43.75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>650</v>
+        <v>6.25</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>6.25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3.8</v>
+        <v>230</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1"/>
+      <c r="B18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>900</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>295</v>
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>700</v>
+        <v>3.8</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>3.8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="A21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>295</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="B23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="n">
+        <v>1301</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1301</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>1301</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>295</v>
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>700</v>
+        <v>10.16</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>10.16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>0.75</v>
-      </c>
+      <c r="A26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1301</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>1301</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <f aca="false">D$9+(D15*(1/D$8)*(1/9.8))</f>
-        <v>3.8843537414966</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="3" t="n">
-        <f aca="false">D15+PI()*(D17*(1/100)*(1/2))^2*101325</f>
-        <v>764.91419710062</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <f aca="false">D32*(1/4.448)/D14</f>
-        <v>0.747687477616339</v>
-      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="4" t="n">
-        <f aca="false">D33*D$7/(D$7+1)</f>
-        <v>0.654226542914297</v>
+        <v>17</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <f aca="false">G$12+(G18*(1/G$11)*(1/9.8))</f>
+        <v>4.22448979591837</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,191 +806,371 @@
         <v>31</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="4" t="n">
-        <f aca="false">D33/(D$7+1)</f>
-        <v>0.0934609347020424</v>
+        <v>26</v>
+      </c>
+      <c r="D35" s="8" t="n">
+        <f aca="false">D18+PI()*(D20*(1/100)*(1/2))^2*101325</f>
+        <v>1014.91419710062</v>
+      </c>
+      <c r="E35" s="8" t="n">
+        <f aca="false">E18+PI()*(E20*(1/100)*(1/2))^2*101325</f>
+        <v>1014.91419710062</v>
+      </c>
+      <c r="G35" s="8" t="n">
+        <f aca="false">G18+PI()*(G20*(1/100)*(1/2))^2*101325</f>
+        <v>1014.91419710062</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <f aca="false">D$11*D16</f>
-        <v>48.23</v>
+        <v>35</v>
+      </c>
+      <c r="D36" s="9" t="n">
+        <f aca="false">D35*(1/4.448)/D17</f>
+        <v>0.992057199230353</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <f aca="false">E35*(1/4.448)/E17</f>
+        <v>0.992057199230353</v>
+      </c>
+      <c r="G36" s="9" t="n">
+        <f aca="false">G35*(1/4.448)/G17</f>
+        <v>0.992057199230353</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <f aca="false">D$12*D16</f>
-        <v>6.89</v>
+        <v>35</v>
+      </c>
+      <c r="D37" s="9" t="n">
+        <f aca="false">D36*D$10/(D$10+1)</f>
+        <v>0.868050049326559</v>
+      </c>
+      <c r="E37" s="9" t="n">
+        <f aca="false">E36*E$10/(E$10+1)</f>
+        <v>0.868050049326559</v>
+      </c>
+      <c r="G37" s="9" t="n">
+        <f aca="false">G36*G$10/(G$10+1)</f>
+        <v>0.868050049326559</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2"/>
+      <c r="B38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="9" t="n">
+        <f aca="false">D36/(D$10+1)</f>
+        <v>0.124007149903794</v>
+      </c>
+      <c r="E38" s="9" t="n">
+        <f aca="false">E36/(E$10+1)</f>
+        <v>0.124007149903794</v>
+      </c>
+      <c r="G38" s="9" t="n">
+        <f aca="false">G36/(G$10+1)</f>
+        <v>0.124007149903794</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <f aca="false">D$9+(D20/D$8/9.8)</f>
-        <v>3.95238095238095</v>
+        <v>17</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <f aca="false">D$14*D19</f>
+        <v>21.875</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <f aca="false">E$14*E19</f>
+        <v>21.875</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <f aca="false">G$14*G19</f>
+        <v>21.875</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="4" t="n">
-        <f aca="false">D20*(1/4.448)/D19</f>
-        <v>0.533471527862456</v>
+        <v>17</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <f aca="false">D$15*D19</f>
+        <v>3.125</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <f aca="false">E$15*E19</f>
+        <v>3.125</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <f aca="false">G$15*G19</f>
+        <v>3.125</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="A41" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="4" t="n">
-        <f aca="false">D40*D$7/(D$7+1)</f>
-        <v>0.466787586879649</v>
-      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="4" t="n">
-        <f aca="false">D40/(D$7+1)</f>
-        <v>0.066683940982807</v>
+        <v>17</v>
+      </c>
+      <c r="D42" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G42" s="7" t="n">
+        <f aca="false">G$12+(G23/G$11/9.8)</f>
+        <v>4.77006802721088</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <f aca="false">D$11*D21</f>
-        <v>48.23</v>
+        <v>35</v>
+      </c>
+      <c r="D43" s="9" t="n">
+        <f aca="false">D23*(1/4.448)/D22</f>
+        <v>0.991494939641507</v>
+      </c>
+      <c r="E43" s="9" t="n">
+        <f aca="false">E23*(1/4.448)/E22</f>
+        <v>0.991494939641507</v>
+      </c>
+      <c r="G43" s="9" t="n">
+        <f aca="false">G23*(1/4.448)/G22</f>
+        <v>0.991494939641507</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <f aca="false">D$12*D21</f>
-        <v>6.89</v>
+        <v>35</v>
+      </c>
+      <c r="D44" s="9" t="n">
+        <f aca="false">D43*D$10/(D$10+1)</f>
+        <v>0.867558072186319</v>
+      </c>
+      <c r="E44" s="9" t="n">
+        <f aca="false">E43*E$10/(E$10+1)</f>
+        <v>0.867558072186319</v>
+      </c>
+      <c r="G44" s="9" t="n">
+        <f aca="false">G43*G$10/(G$10+1)</f>
+        <v>0.867558072186319</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="2"/>
+      <c r="B45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="9" t="n">
+        <f aca="false">D43/(D$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
+      <c r="E45" s="9" t="n">
+        <f aca="false">E43/(E$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
+      <c r="G45" s="9" t="n">
+        <f aca="false">G43/(G$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <f aca="false">D$9+(D25/D$8/9.8)</f>
-        <v>3.95238095238095</v>
+        <v>17</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <f aca="false">D$14*D24</f>
+        <v>21.875</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <f aca="false">E$14*E24</f>
+        <v>21.875</v>
+      </c>
+      <c r="G46" s="5" t="n">
+        <f aca="false">G$14*G24</f>
+        <v>21.875</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="4" t="n">
-        <f aca="false">D25*(1/4.448)/D24</f>
-        <v>0.533471527862456</v>
+        <v>17</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <f aca="false">D$15*D24</f>
+        <v>3.125</v>
+      </c>
+      <c r="E47" s="5" t="n">
+        <f aca="false">E$15*E24</f>
+        <v>3.125</v>
+      </c>
+      <c r="G47" s="5" t="n">
+        <f aca="false">G$15*G24</f>
+        <v>3.125</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="4" t="n">
-        <f aca="false">D47*D$7/(D$7+1)</f>
-        <v>0.466787586879649</v>
-      </c>
+      <c r="A48" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="4" t="n">
-        <f aca="false">D47/(D$7+1)</f>
-        <v>0.066683940982807</v>
+        <v>17</v>
+      </c>
+      <c r="D49" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E49" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G49" s="7" t="n">
+        <f aca="false">G$12+(G28/G$11/9.8)</f>
+        <v>4.77006802721088</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <f aca="false">D$11*D26</f>
-        <v>72.345</v>
+        <v>35</v>
+      </c>
+      <c r="D50" s="9" t="n">
+        <f aca="false">D28*(1/4.448)/D27</f>
+        <v>0.991494939641507</v>
+      </c>
+      <c r="E50" s="9" t="n">
+        <f aca="false">E28*(1/4.448)/E27</f>
+        <v>0.991494939641507</v>
+      </c>
+      <c r="G50" s="9" t="n">
+        <f aca="false">G28*(1/4.448)/G27</f>
+        <v>0.991494939641507</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <f aca="false">D$12*D26</f>
-        <v>10.335</v>
+        <v>35</v>
+      </c>
+      <c r="D51" s="9" t="n">
+        <f aca="false">D50*D$10/(D$10+1)</f>
+        <v>0.867558072186319</v>
+      </c>
+      <c r="E51" s="9" t="n">
+        <f aca="false">E50*E$10/(E$10+1)</f>
+        <v>0.867558072186319</v>
+      </c>
+      <c r="G51" s="9" t="n">
+        <f aca="false">G50*G$10/(G$10+1)</f>
+        <v>0.867558072186319</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="9" t="n">
+        <f aca="false">D50/(D$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
+      <c r="E52" s="9" t="n">
+        <f aca="false">E50/(E$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
+      <c r="G52" s="9" t="n">
+        <f aca="false">G50/(G$10+1)</f>
+        <v>0.123936867455188</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="5" t="n">
+        <f aca="false">D$14*D29</f>
+        <v>21.875</v>
+      </c>
+      <c r="E53" s="5" t="n">
+        <f aca="false">E$14*E29</f>
+        <v>32.8125</v>
+      </c>
+      <c r="G53" s="5" t="n">
+        <f aca="false">G$14*G29</f>
+        <v>32.8125</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <f aca="false">D$15*D29</f>
+        <v>3.125</v>
+      </c>
+      <c r="E54" s="5" t="n">
+        <f aca="false">E$15*E29</f>
+        <v>4.6875</v>
+      </c>
+      <c r="G54" s="5" t="n">
+        <f aca="false">G$15*G29</f>
+        <v>4.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PB1-6.1 control system tuning misc script tweaks
</commit_message>
<xml_diff>
--- a/configurations.xlsx
+++ b/configurations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Notes: red is input parameter, black font is calculated parameter, yellow highlights changed parameters</t>
   </si>
@@ -64,6 +64,9 @@
     <t>PB1-5.4</t>
   </si>
   <si>
+    <t>PB1-6.1</t>
+  </si>
+  <si>
     <t>perigee x apogee (miles)</t>
   </si>
   <si>
@@ -98,6 +101,9 @@
   </si>
   <si>
     <t>stage3 only engine mass comparison</t>
+  </si>
+  <si>
+    <t>controls tuning, high fill and low thrust</t>
   </si>
   <si>
     <t>created</t>
@@ -279,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -317,10 +323,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,19 +423,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" ySplit="0" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topRight" activeCell="U6" activeCellId="0" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.48469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.64285714285714"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -482,55 +484,74 @@
       <c r="S4" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="U4" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>173.9</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="L5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>202.8</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="U5" s="2" t="n">
+        <v>-331.6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>42459</v>
@@ -571,10 +592,13 @@
       <c r="S7" s="4" t="n">
         <v>42461</v>
       </c>
+      <c r="U7" s="4" t="n">
+        <v>42462</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>42459</v>
@@ -583,8 +607,12 @@
       <c r="F8" s="4" t="n">
         <v>42459</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="4" t="n">
+        <v>42461</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>42461</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="L8" s="4" t="n">
@@ -600,21 +628,25 @@
       <c r="P8" s="4" t="n">
         <v>42461</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="Q8" s="4" t="n">
+        <v>42461</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>42461</v>
+      </c>
       <c r="S8" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>7</v>
@@ -657,13 +689,16 @@
         <v>7</v>
       </c>
       <c r="T11" s="5"/>
+      <c r="U11" s="5" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>75</v>
@@ -706,13 +741,16 @@
         <v>75</v>
       </c>
       <c r="T12" s="5"/>
+      <c r="U12" s="5" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>3</v>
@@ -755,13 +793,16 @@
         <v>3</v>
       </c>
       <c r="T13" s="5"/>
+      <c r="U13" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>4</v>
@@ -804,13 +845,16 @@
         <v>4</v>
       </c>
       <c r="T14" s="5"/>
+      <c r="U14" s="5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>43.75</v>
@@ -853,13 +897,16 @@
         <v>43.75</v>
       </c>
       <c r="T15" s="5"/>
+      <c r="U15" s="5" t="n">
+        <v>43.75</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>6.25</v>
@@ -902,10 +949,13 @@
         <v>6.25</v>
       </c>
       <c r="T16" s="5"/>
+      <c r="U16" s="5" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -924,13 +974,14 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>230</v>
@@ -973,13 +1024,16 @@
         <v>230</v>
       </c>
       <c r="T18" s="5"/>
+      <c r="U18" s="5" t="n">
+        <v>230</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>900</v>
@@ -1022,13 +1076,16 @@
         <v>900</v>
       </c>
       <c r="T19" s="5"/>
+      <c r="U19" s="5" t="n">
+        <v>900</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>0.5</v>
@@ -1071,13 +1128,16 @@
         <v>0.5</v>
       </c>
       <c r="T20" s="5"/>
+      <c r="U20" s="5" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>3.8</v>
@@ -1120,10 +1180,13 @@
         <v>3.8</v>
       </c>
       <c r="T21" s="5"/>
+      <c r="U21" s="5" t="n">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1142,13 +1205,14 @@
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>295</v>
@@ -1191,13 +1255,16 @@
         <v>295</v>
       </c>
       <c r="T23" s="5"/>
+      <c r="U23" s="5" t="n">
+        <v>295</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>1301</v>
@@ -1240,13 +1307,16 @@
         <v>1200</v>
       </c>
       <c r="T24" s="5"/>
+      <c r="U24" s="5" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>0.5</v>
@@ -1289,13 +1359,16 @@
         <v>0.5</v>
       </c>
       <c r="T25" s="5"/>
+      <c r="U25" s="5" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>10.16</v>
@@ -1338,10 +1411,13 @@
         <v>10.16</v>
       </c>
       <c r="T26" s="5"/>
+      <c r="U26" s="5" t="n">
+        <v>10.16</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -1360,13 +1436,14 @@
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>295</v>
@@ -1409,13 +1486,16 @@
         <v>295</v>
       </c>
       <c r="T28" s="5"/>
+      <c r="U28" s="5" t="n">
+        <v>295</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>1301</v>
@@ -1458,13 +1538,16 @@
         <v>800</v>
       </c>
       <c r="T29" s="5"/>
+      <c r="U29" s="6" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>0.5</v>
@@ -1507,13 +1590,16 @@
         <v>0.75</v>
       </c>
       <c r="T30" s="5"/>
+      <c r="U30" s="6" t="n">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>10.16</v>
@@ -1556,6 +1642,9 @@
         <v>10.16</v>
       </c>
       <c r="T31" s="5"/>
+      <c r="U31" s="5" t="n">
+        <v>10.16</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O32" s="1"/>
@@ -1565,7 +1654,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1582,13 +1671,14 @@
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
+      <c r="U34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>4.4</v>
@@ -1607,15 +1697,15 @@
         <v>4.4</v>
       </c>
       <c r="J35" s="9"/>
-      <c r="L35" s="10" t="n">
+      <c r="L35" s="7" t="n">
         <f aca="false">L$13+(L19*(1/L$12)*(1/9.8))</f>
         <v>4.22448979591837</v>
       </c>
-      <c r="M35" s="10" t="n">
+      <c r="M35" s="7" t="n">
         <f aca="false">M$13+(M19*(1/M$12)*(1/9.8))</f>
         <v>4.22448979591837</v>
       </c>
-      <c r="N35" s="10" t="n">
+      <c r="N35" s="7" t="n">
         <f aca="false">N$13+(N19*(1/N$12)*(1/9.8))</f>
         <v>4.22448979591837</v>
       </c>
@@ -1636,249 +1726,269 @@
         <f aca="false">S$13+(S19*(1/S$12)*(1/9.8))</f>
         <v>4.22448979591837</v>
       </c>
+      <c r="U35" s="7" t="n">
+        <f aca="false">U$13+(U19*(1/U$12)*(1/9.8))</f>
+        <v>4.22448979591837</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="D36" s="10" t="n">
         <f aca="false">D19+PI()*(D21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11" t="n">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="n">
         <f aca="false">F19+PI()*(F21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="G36" s="11" t="n">
+      <c r="G36" s="10" t="n">
         <f aca="false">G19+PI()*(G21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="H36" s="11" t="n">
+      <c r="H36" s="10" t="n">
         <f aca="false">H19+PI()*(H21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="I36" s="11" t="n">
+      <c r="I36" s="10" t="n">
         <f aca="false">I19+PI()*(I21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="L36" s="11" t="n">
+      <c r="J36" s="10"/>
+      <c r="L36" s="10" t="n">
         <f aca="false">L19+PI()*(L21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="M36" s="11" t="n">
+      <c r="M36" s="10" t="n">
         <f aca="false">M19+PI()*(M21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="N36" s="11" t="n">
+      <c r="N36" s="10" t="n">
         <f aca="false">N19+PI()*(N21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="O36" s="12"/>
-      <c r="P36" s="11" t="n">
+      <c r="O36" s="11"/>
+      <c r="P36" s="10" t="n">
         <f aca="false">P19+PI()*(P21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="Q36" s="11" t="n">
+      <c r="Q36" s="10" t="n">
         <f aca="false">Q19+PI()*(Q21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="R36" s="11" t="n">
+      <c r="R36" s="10" t="n">
         <f aca="false">R19+PI()*(R21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
-      <c r="S36" s="11" t="n">
+      <c r="S36" s="10" t="n">
         <f aca="false">S19+PI()*(S21*(1/100)*(1/2))^2*101325</f>
         <v>1014.91419710062</v>
       </c>
+      <c r="U36" s="10" t="n">
+        <f aca="false">U19+PI()*(U21*(1/100)*(1/2))^2*101325</f>
+        <v>1014.91419710062</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D37" s="12" t="n">
         <f aca="false">D36*(1/4.448)/D18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13" t="n">
+      <c r="E37" s="12"/>
+      <c r="F37" s="12" t="n">
         <f aca="false">F36*(1/4.448)/F18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="G37" s="13" t="n">
+      <c r="G37" s="12" t="n">
         <f aca="false">G36*(1/4.448)/G18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="H37" s="13" t="n">
+      <c r="H37" s="12" t="n">
         <f aca="false">H36*(1/4.448)/H18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="I37" s="13" t="n">
+      <c r="I37" s="12" t="n">
         <f aca="false">I36*(1/4.448)/I18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="J37" s="13"/>
-      <c r="L37" s="13" t="n">
+      <c r="J37" s="12"/>
+      <c r="L37" s="12" t="n">
         <f aca="false">L36*(1/4.448)/L18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="M37" s="13" t="n">
+      <c r="M37" s="12" t="n">
         <f aca="false">M36*(1/4.448)/M18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="N37" s="13" t="n">
+      <c r="N37" s="12" t="n">
         <f aca="false">N36*(1/4.448)/N18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="O37" s="14"/>
-      <c r="P37" s="13" t="n">
+      <c r="O37" s="13"/>
+      <c r="P37" s="12" t="n">
         <f aca="false">P36*(1/4.448)/P18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="Q37" s="13" t="n">
+      <c r="Q37" s="12" t="n">
         <f aca="false">Q36*(1/4.448)/Q18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="R37" s="13" t="n">
+      <c r="R37" s="12" t="n">
         <f aca="false">R36*(1/4.448)/R18</f>
         <v>0.992057199230353</v>
       </c>
-      <c r="S37" s="13" t="n">
+      <c r="S37" s="12" t="n">
         <f aca="false">S36*(1/4.448)/S18</f>
         <v>0.992057199230353</v>
       </c>
+      <c r="U37" s="12" t="n">
+        <f aca="false">U36*(1/4.448)/U18</f>
+        <v>0.992057199230353</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D38" s="12" t="n">
         <f aca="false">D37*D$11/(D$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13" t="n">
+      <c r="E38" s="12"/>
+      <c r="F38" s="12" t="n">
         <f aca="false">F37*F$11/(F$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="G38" s="13" t="n">
+      <c r="G38" s="12" t="n">
         <f aca="false">G37*G$11/(G$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="H38" s="13" t="n">
+      <c r="H38" s="12" t="n">
         <f aca="false">H37*H$11/(H$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="I38" s="13" t="n">
+      <c r="I38" s="12" t="n">
         <f aca="false">I37*I$11/(I$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="J38" s="13"/>
-      <c r="L38" s="13" t="n">
+      <c r="J38" s="12"/>
+      <c r="L38" s="12" t="n">
         <f aca="false">L37*L$11/(L$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="M38" s="13" t="n">
+      <c r="M38" s="12" t="n">
         <f aca="false">M37*M$11/(M$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="N38" s="13" t="n">
+      <c r="N38" s="12" t="n">
         <f aca="false">N37*N$11/(N$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13" t="n">
+      <c r="O38" s="12"/>
+      <c r="P38" s="12" t="n">
         <f aca="false">P37*P$11/(P$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="Q38" s="13" t="n">
+      <c r="Q38" s="12" t="n">
         <f aca="false">Q37*Q$11/(Q$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="R38" s="13" t="n">
+      <c r="R38" s="12" t="n">
         <f aca="false">R37*R$11/(R$11+1)</f>
         <v>0.868050049326559</v>
       </c>
-      <c r="S38" s="13" t="n">
+      <c r="S38" s="12" t="n">
         <f aca="false">S37*S$11/(S$11+1)</f>
         <v>0.868050049326559</v>
       </c>
+      <c r="U38" s="12" t="n">
+        <f aca="false">U37*U$11/(U$11+1)</f>
+        <v>0.868050049326559</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="13" t="n">
+      <c r="D39" s="12" t="n">
         <f aca="false">D37/(D$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13" t="n">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="n">
         <f aca="false">F37/(F$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="G39" s="13" t="n">
+      <c r="G39" s="12" t="n">
         <f aca="false">G37/(G$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="H39" s="13" t="n">
+      <c r="H39" s="12" t="n">
         <f aca="false">H37/(H$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="I39" s="13" t="n">
+      <c r="I39" s="12" t="n">
         <f aca="false">I37/(I$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="J39" s="13"/>
-      <c r="L39" s="13" t="n">
+      <c r="J39" s="12"/>
+      <c r="L39" s="12" t="n">
         <f aca="false">L37/(L$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="M39" s="13" t="n">
+      <c r="M39" s="12" t="n">
         <f aca="false">M37/(M$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="N39" s="13" t="n">
+      <c r="N39" s="12" t="n">
         <f aca="false">N37/(N$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13" t="n">
+      <c r="O39" s="12"/>
+      <c r="P39" s="12" t="n">
         <f aca="false">P37/(P$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="Q39" s="13" t="n">
+      <c r="Q39" s="12" t="n">
         <f aca="false">Q37/(Q$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="R39" s="13" t="n">
+      <c r="R39" s="12" t="n">
         <f aca="false">R37/(R$11+1)</f>
         <v>0.124007149903794</v>
       </c>
-      <c r="S39" s="13" t="n">
+      <c r="S39" s="12" t="n">
         <f aca="false">S37/(S$11+1)</f>
         <v>0.124007149903794</v>
       </c>
+      <c r="U39" s="12" t="n">
+        <f aca="false">U37/(U$11+1)</f>
+        <v>0.124007149903794</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D40" s="7" t="n">
         <f aca="false">D$15*D20</f>
@@ -1931,13 +2041,17 @@
         <f aca="false">S$15*S20</f>
         <v>21.875</v>
       </c>
+      <c r="U40" s="7" t="n">
+        <f aca="false">U$15*U20</f>
+        <v>21.875</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D41" s="7" t="n">
         <f aca="false">D$16*D20</f>
@@ -1990,10 +2104,14 @@
         <f aca="false">S$16*S20</f>
         <v>3.125</v>
       </c>
+      <c r="U41" s="7" t="n">
+        <f aca="false">U$16*U20</f>
+        <v>3.125</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -2010,13 +2128,14 @@
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
+      <c r="U42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D43" s="9" t="n">
         <v>4.4</v>
@@ -2035,15 +2154,15 @@
         <v>4.4</v>
       </c>
       <c r="J43" s="9"/>
-      <c r="L43" s="15" t="n">
+      <c r="L43" s="14" t="n">
         <f aca="false">L$13+(L24/L$12/9.8)</f>
         <v>4.77006802721088</v>
       </c>
-      <c r="M43" s="15" t="n">
+      <c r="M43" s="14" t="n">
         <f aca="false">M$13+(M24/M$12/9.8)</f>
         <v>4.63265306122449</v>
       </c>
-      <c r="N43" s="15" t="n">
+      <c r="N43" s="14" t="n">
         <f aca="false">N$13+(N24/N$12/9.8)</f>
         <v>4.49659863945578</v>
       </c>
@@ -2064,190 +2183,206 @@
         <f aca="false">S$13+(S24/S$12/9.8)</f>
         <v>4.63265306122449</v>
       </c>
+      <c r="U43" s="7" t="n">
+        <f aca="false">U$13+(U24/U$12/9.8)</f>
+        <v>4.63265306122449</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D44" s="12" t="n">
         <f aca="false">D24*(1/4.448)/D23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13" t="n">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12" t="n">
         <f aca="false">F24*(1/4.448)/F23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="G44" s="13" t="n">
+      <c r="G44" s="12" t="n">
         <f aca="false">G24*(1/4.448)/G23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="H44" s="13" t="n">
+      <c r="H44" s="12" t="n">
         <f aca="false">H24*(1/4.448)/H23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="I44" s="13" t="n">
+      <c r="I44" s="12" t="n">
         <f aca="false">I24*(1/4.448)/I23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="J44" s="13"/>
-      <c r="L44" s="13" t="n">
+      <c r="J44" s="12"/>
+      <c r="L44" s="12" t="n">
         <f aca="false">L24*(1/4.448)/L23</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="M44" s="13" t="n">
+      <c r="M44" s="12" t="n">
         <f aca="false">M24*(1/4.448)/M23</f>
         <v>0.914522619192781</v>
       </c>
-      <c r="N44" s="13" t="n">
+      <c r="N44" s="12" t="n">
         <f aca="false">N24*(1/4.448)/N23</f>
         <v>0.838312400926716</v>
       </c>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13" t="n">
+      <c r="O44" s="12"/>
+      <c r="P44" s="12" t="n">
         <f aca="false">P24*(1/4.448)/P23</f>
         <v>0.914522619192781</v>
       </c>
-      <c r="Q44" s="13" t="n">
+      <c r="Q44" s="12" t="n">
         <f aca="false">Q24*(1/4.448)/Q23</f>
         <v>0.914522619192781</v>
       </c>
-      <c r="R44" s="13" t="n">
+      <c r="R44" s="12" t="n">
         <f aca="false">R24*(1/4.448)/R23</f>
         <v>0.914522619192781</v>
       </c>
-      <c r="S44" s="13" t="n">
+      <c r="S44" s="12" t="n">
         <f aca="false">S24*(1/4.448)/S23</f>
         <v>0.914522619192781</v>
       </c>
+      <c r="U44" s="12" t="n">
+        <f aca="false">U24*(1/4.448)/U23</f>
+        <v>0.914522619192781</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D45" s="12" t="n">
         <f aca="false">D44*D$11/(D$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13" t="n">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12" t="n">
         <f aca="false">F44*F$11/(F$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="G45" s="13" t="n">
+      <c r="G45" s="12" t="n">
         <f aca="false">G44*G$11/(G$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="H45" s="13" t="n">
+      <c r="H45" s="12" t="n">
         <f aca="false">H44*H$11/(H$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="I45" s="13" t="n">
+      <c r="I45" s="12" t="n">
         <f aca="false">I44*I$11/(I$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="J45" s="13"/>
-      <c r="L45" s="13" t="n">
+      <c r="J45" s="12"/>
+      <c r="L45" s="12" t="n">
         <f aca="false">L44*L$11/(L$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="M45" s="13" t="n">
+      <c r="M45" s="12" t="n">
         <f aca="false">M44*M$11/(M$11+1)</f>
         <v>0.800207291793684</v>
       </c>
-      <c r="N45" s="13" t="n">
+      <c r="N45" s="12" t="n">
         <f aca="false">N44*N$11/(N$11+1)</f>
         <v>0.733523350810877</v>
       </c>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13" t="n">
+      <c r="O45" s="12"/>
+      <c r="P45" s="12" t="n">
         <f aca="false">P44*P$11/(P$11+1)</f>
         <v>0.800207291793684</v>
       </c>
-      <c r="Q45" s="13" t="n">
+      <c r="Q45" s="12" t="n">
         <f aca="false">Q44*Q$11/(Q$11+1)</f>
         <v>0.800207291793684</v>
       </c>
-      <c r="R45" s="13" t="n">
+      <c r="R45" s="12" t="n">
         <f aca="false">R44*R$11/(R$11+1)</f>
         <v>0.800207291793684</v>
       </c>
-      <c r="S45" s="13" t="n">
+      <c r="S45" s="12" t="n">
         <f aca="false">S44*S$11/(S$11+1)</f>
         <v>0.800207291793684</v>
       </c>
+      <c r="U45" s="12" t="n">
+        <f aca="false">U44*U$11/(U$11+1)</f>
+        <v>0.800207291793684</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="13" t="n">
+      <c r="D46" s="12" t="n">
         <f aca="false">D44/(D$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13" t="n">
+      <c r="E46" s="12"/>
+      <c r="F46" s="12" t="n">
         <f aca="false">F44/(F$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="G46" s="13" t="n">
+      <c r="G46" s="12" t="n">
         <f aca="false">G44/(G$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="H46" s="13" t="n">
+      <c r="H46" s="12" t="n">
         <f aca="false">H44/(H$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="I46" s="13" t="n">
+      <c r="I46" s="12" t="n">
         <f aca="false">I44/(I$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="J46" s="13"/>
-      <c r="L46" s="13" t="n">
+      <c r="J46" s="12"/>
+      <c r="L46" s="12" t="n">
         <f aca="false">L44/(L$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="M46" s="13" t="n">
+      <c r="M46" s="12" t="n">
         <f aca="false">M44/(M$11+1)</f>
         <v>0.114315327399098</v>
       </c>
-      <c r="N46" s="13" t="n">
+      <c r="N46" s="12" t="n">
         <f aca="false">N44/(N$11+1)</f>
         <v>0.10478905011584</v>
       </c>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13" t="n">
+      <c r="O46" s="12"/>
+      <c r="P46" s="12" t="n">
         <f aca="false">P44/(P$11+1)</f>
         <v>0.114315327399098</v>
       </c>
-      <c r="Q46" s="13" t="n">
+      <c r="Q46" s="12" t="n">
         <f aca="false">Q44/(Q$11+1)</f>
         <v>0.114315327399098</v>
       </c>
-      <c r="R46" s="13" t="n">
+      <c r="R46" s="12" t="n">
         <f aca="false">R44/(R$11+1)</f>
         <v>0.114315327399098</v>
       </c>
-      <c r="S46" s="13" t="n">
+      <c r="S46" s="12" t="n">
         <f aca="false">S44/(S$11+1)</f>
         <v>0.114315327399098</v>
       </c>
+      <c r="U46" s="12" t="n">
+        <f aca="false">U44/(U$11+1)</f>
+        <v>0.114315327399098</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D47" s="7" t="n">
         <f aca="false">D$15*D25</f>
@@ -2300,13 +2435,17 @@
         <f aca="false">S$15*S25</f>
         <v>21.875</v>
       </c>
+      <c r="U47" s="7" t="n">
+        <f aca="false">U$15*U25</f>
+        <v>21.875</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D48" s="7" t="n">
         <f aca="false">D$16*D25</f>
@@ -2359,10 +2498,14 @@
         <f aca="false">S$16*S25</f>
         <v>3.125</v>
       </c>
+      <c r="U48" s="7" t="n">
+        <f aca="false">U$16*U25</f>
+        <v>3.125</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -2379,13 +2522,14 @@
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
       <c r="S49" s="7"/>
+      <c r="U49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D50" s="9" t="n">
         <v>4.4</v>
@@ -2404,219 +2548,235 @@
         <v>4.4</v>
       </c>
       <c r="J50" s="9"/>
-      <c r="L50" s="15" t="n">
+      <c r="L50" s="14" t="n">
         <f aca="false">L$13+(L29/L$12/9.8)</f>
         <v>4.77006802721088</v>
       </c>
-      <c r="M50" s="15" t="n">
+      <c r="M50" s="14" t="n">
         <f aca="false">M$13+(M29/M$12/9.8)</f>
         <v>4.63265306122449</v>
       </c>
-      <c r="N50" s="15" t="n">
+      <c r="N50" s="14" t="n">
         <f aca="false">N$13+(N29/N$12/9.8)</f>
         <v>4.49659863945578</v>
       </c>
       <c r="O50" s="7"/>
-      <c r="P50" s="15" t="n">
+      <c r="P50" s="14" t="n">
         <f aca="false">P$13+(P29/P$12/9.8)</f>
         <v>4.49659863945578</v>
       </c>
-      <c r="Q50" s="15" t="n">
+      <c r="Q50" s="14" t="n">
         <f aca="false">Q$13+(Q29/Q$12/9.8)</f>
         <v>4.36054421768707</v>
       </c>
-      <c r="R50" s="15" t="n">
+      <c r="R50" s="14" t="n">
         <f aca="false">R$13+(R29/R$12/9.8)</f>
         <v>4.22448979591837</v>
       </c>
-      <c r="S50" s="15" t="n">
+      <c r="S50" s="14" t="n">
         <f aca="false">S$13+(S29/S$12/9.8)</f>
         <v>4.08843537414966</v>
       </c>
+      <c r="U50" s="7" t="n">
+        <f aca="false">U$13+(U29/U$12/9.8)</f>
+        <v>4.36054421768707</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D51" s="12" t="n">
         <f aca="false">D29*(1/4.448)/D28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13" t="n">
+      <c r="E51" s="12"/>
+      <c r="F51" s="12" t="n">
         <f aca="false">F29*(1/4.448)/F28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="G51" s="13" t="n">
+      <c r="G51" s="12" t="n">
         <f aca="false">G29*(1/4.448)/G28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="H51" s="13" t="n">
+      <c r="H51" s="12" t="n">
         <f aca="false">H29*(1/4.448)/H28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="I51" s="13" t="n">
+      <c r="I51" s="12" t="n">
         <f aca="false">I29*(1/4.448)/I28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="J51" s="13"/>
-      <c r="L51" s="13" t="n">
+      <c r="J51" s="12"/>
+      <c r="L51" s="12" t="n">
         <f aca="false">L29*(1/4.448)/L28</f>
         <v>0.991494939641507</v>
       </c>
-      <c r="M51" s="13" t="n">
+      <c r="M51" s="12" t="n">
         <f aca="false">M29*(1/4.448)/M28</f>
         <v>0.914522619192781</v>
       </c>
-      <c r="N51" s="13" t="n">
+      <c r="N51" s="12" t="n">
         <f aca="false">N29*(1/4.448)/N28</f>
         <v>0.838312400926716</v>
       </c>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13" t="n">
+      <c r="O51" s="12"/>
+      <c r="P51" s="12" t="n">
         <f aca="false">P29*(1/4.448)/P28</f>
         <v>0.838312400926716</v>
       </c>
-      <c r="Q51" s="13" t="n">
+      <c r="Q51" s="12" t="n">
         <f aca="false">Q29*(1/4.448)/Q28</f>
         <v>0.762102182660651</v>
       </c>
-      <c r="R51" s="13" t="n">
+      <c r="R51" s="12" t="n">
         <f aca="false">R29*(1/4.448)/R28</f>
         <v>0.685891964394586</v>
       </c>
-      <c r="S51" s="13" t="n">
+      <c r="S51" s="12" t="n">
         <f aca="false">S29*(1/4.448)/S28</f>
         <v>0.609681746128521</v>
       </c>
+      <c r="U51" s="12" t="n">
+        <f aca="false">U29*(1/4.448)/U28</f>
+        <v>0.762102182660651</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="D52" s="12" t="n">
         <f aca="false">D51*D$11/(D$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13" t="n">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12" t="n">
         <f aca="false">F51*F$11/(F$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="G52" s="13" t="n">
+      <c r="G52" s="12" t="n">
         <f aca="false">G51*G$11/(G$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="H52" s="13" t="n">
+      <c r="H52" s="12" t="n">
         <f aca="false">H51*H$11/(H$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="I52" s="13" t="n">
+      <c r="I52" s="12" t="n">
         <f aca="false">I51*I$11/(I$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="J52" s="13"/>
-      <c r="L52" s="13" t="n">
+      <c r="J52" s="12"/>
+      <c r="L52" s="12" t="n">
         <f aca="false">L51*L$11/(L$11+1)</f>
         <v>0.867558072186319</v>
       </c>
-      <c r="M52" s="13" t="n">
+      <c r="M52" s="12" t="n">
         <f aca="false">M51*M$11/(M$11+1)</f>
         <v>0.800207291793684</v>
       </c>
-      <c r="N52" s="13" t="n">
+      <c r="N52" s="12" t="n">
         <f aca="false">N51*N$11/(N$11+1)</f>
         <v>0.733523350810877</v>
       </c>
-      <c r="O52" s="13"/>
-      <c r="P52" s="13" t="n">
+      <c r="O52" s="12"/>
+      <c r="P52" s="12" t="n">
         <f aca="false">P51*P$11/(P$11+1)</f>
         <v>0.733523350810877</v>
       </c>
-      <c r="Q52" s="13" t="n">
+      <c r="Q52" s="12" t="n">
         <f aca="false">Q51*Q$11/(Q$11+1)</f>
         <v>0.66683940982807</v>
       </c>
-      <c r="R52" s="13" t="n">
+      <c r="R52" s="12" t="n">
         <f aca="false">R51*R$11/(R$11+1)</f>
         <v>0.600155468845263</v>
       </c>
-      <c r="S52" s="13" t="n">
+      <c r="S52" s="12" t="n">
         <f aca="false">S51*S$11/(S$11+1)</f>
         <v>0.533471527862456</v>
       </c>
+      <c r="U52" s="12" t="n">
+        <f aca="false">U51*U$11/(U$11+1)</f>
+        <v>0.66683940982807</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="13" t="n">
+      <c r="D53" s="12" t="n">
         <f aca="false">D51/(D$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13" t="n">
+      <c r="E53" s="12"/>
+      <c r="F53" s="12" t="n">
         <f aca="false">F51/(F$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="G53" s="13" t="n">
+      <c r="G53" s="12" t="n">
         <f aca="false">G51/(G$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="H53" s="13" t="n">
+      <c r="H53" s="12" t="n">
         <f aca="false">H51/(H$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="I53" s="13" t="n">
+      <c r="I53" s="12" t="n">
         <f aca="false">I51/(I$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="J53" s="13"/>
-      <c r="L53" s="13" t="n">
+      <c r="J53" s="12"/>
+      <c r="L53" s="12" t="n">
         <f aca="false">L51/(L$11+1)</f>
         <v>0.123936867455188</v>
       </c>
-      <c r="M53" s="13" t="n">
+      <c r="M53" s="12" t="n">
         <f aca="false">M51/(M$11+1)</f>
         <v>0.114315327399098</v>
       </c>
-      <c r="N53" s="13" t="n">
+      <c r="N53" s="12" t="n">
         <f aca="false">N51/(N$11+1)</f>
         <v>0.10478905011584</v>
       </c>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13" t="n">
+      <c r="O53" s="12"/>
+      <c r="P53" s="12" t="n">
         <f aca="false">P51/(P$11+1)</f>
         <v>0.10478905011584</v>
       </c>
-      <c r="Q53" s="13" t="n">
+      <c r="Q53" s="12" t="n">
         <f aca="false">Q51/(Q$11+1)</f>
         <v>0.0952627728325814</v>
       </c>
-      <c r="R53" s="13" t="n">
+      <c r="R53" s="12" t="n">
         <f aca="false">R51/(R$11+1)</f>
         <v>0.0857364955493233</v>
       </c>
-      <c r="S53" s="13" t="n">
+      <c r="S53" s="12" t="n">
         <f aca="false">S51/(S$11+1)</f>
         <v>0.0762102182660651</v>
       </c>
+      <c r="U53" s="12" t="n">
+        <f aca="false">U51/(U$11+1)</f>
+        <v>0.0952627728325814</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D54" s="7" t="n">
         <f aca="false">D$15*D30</f>
@@ -2669,13 +2829,17 @@
         <f aca="false">S$15*S30</f>
         <v>32.8125</v>
       </c>
+      <c r="U54" s="7" t="n">
+        <f aca="false">U$15*U30</f>
+        <v>37.1875</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D55" s="7" t="n">
         <f aca="false">D$16*D30</f>
@@ -2727,6 +2891,10 @@
       <c r="S55" s="7" t="n">
         <f aca="false">S$16*S30</f>
         <v>4.6875</v>
+      </c>
+      <c r="U55" s="7" t="n">
+        <f aca="false">U$16*U30</f>
+        <v>5.3125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks to roll control documentation for blow-down propellant flow rate
</commit_message>
<xml_diff>
--- a/configurations.xlsx
+++ b/configurations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Notes: red is input parameter, black font is calculated parameter, yellow highlights changed parameters</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>187.6 x 189.4</t>
+  </si>
+  <si>
+    <t>236.6 x 237.5</t>
   </si>
   <si>
     <t>notes</t>
@@ -425,18 +428,17 @@
   </sheetPr>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D20" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="topRight" activeCell="U31" activeCellId="0" sqref="U31"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="U6" activeCellId="0" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,33 +527,33 @@
       <c r="R5" s="2" t="n">
         <v>207.5</v>
       </c>
-      <c r="U5" s="2" t="n">
-        <v>-331.6</v>
+      <c r="U5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>42459</v>
@@ -598,7 +600,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>42459</v>
@@ -638,15 +640,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>7</v>
@@ -695,10 +697,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>75</v>
@@ -747,10 +749,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>3</v>
@@ -799,10 +801,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>4</v>
@@ -851,10 +853,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>43.75</v>
@@ -903,10 +905,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>6.25</v>
@@ -955,7 +957,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -978,10 +980,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>230</v>
@@ -1030,10 +1032,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>900</v>
@@ -1082,10 +1084,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>0.5</v>
@@ -1134,10 +1136,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>3.8</v>
@@ -1186,7 +1188,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1209,10 +1211,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>295</v>
@@ -1261,10 +1263,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>1301</v>
@@ -1313,10 +1315,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>0.5</v>
@@ -1365,10 +1367,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>10.16</v>
@@ -1417,7 +1419,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -1440,10 +1442,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>295</v>
@@ -1492,10 +1494,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>1301</v>
@@ -1544,10 +1546,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>0.5</v>
@@ -1596,10 +1598,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>10.16</v>
@@ -1654,7 +1656,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1675,10 +1677,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>4.4</v>
@@ -1733,10 +1735,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D36" s="10" t="n">
         <f aca="false">D19+PI()*(D21*(1/100)*(1/2))^2*101325</f>
@@ -1796,10 +1798,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" s="12" t="n">
         <f aca="false">D36*(1/4.448)/D18</f>
@@ -1859,10 +1861,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="D38" s="12" t="n">
         <f aca="false">D37*D$11/(D$11+1)</f>
@@ -1922,10 +1924,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D39" s="12" t="n">
         <f aca="false">D37/(D$11+1)</f>
@@ -1985,10 +1987,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D40" s="7" t="n">
         <f aca="false">D$15*D20</f>
@@ -2048,10 +2050,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D41" s="7" t="n">
         <f aca="false">D$16*D20</f>
@@ -2111,7 +2113,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -2132,10 +2134,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D43" s="9" t="n">
         <v>4.4</v>
@@ -2190,10 +2192,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" s="12" t="n">
         <f aca="false">D24*(1/4.448)/D23</f>
@@ -2253,10 +2255,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="D45" s="12" t="n">
         <f aca="false">D44*D$11/(D$11+1)</f>
@@ -2316,10 +2318,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D46" s="12" t="n">
         <f aca="false">D44/(D$11+1)</f>
@@ -2379,10 +2381,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D47" s="7" t="n">
         <f aca="false">D$15*D25</f>
@@ -2442,10 +2444,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D48" s="7" t="n">
         <f aca="false">D$16*D25</f>
@@ -2505,7 +2507,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -2526,10 +2528,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D50" s="9" t="n">
         <v>4.4</v>
@@ -2584,10 +2586,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D51" s="12" t="n">
         <f aca="false">D29*(1/4.448)/D28</f>
@@ -2647,10 +2649,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="D52" s="12" t="n">
         <f aca="false">D51*D$11/(D$11+1)</f>
@@ -2710,10 +2712,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D53" s="12" t="n">
         <f aca="false">D51/(D$11+1)</f>
@@ -2773,10 +2775,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D54" s="7" t="n">
         <f aca="false">D$15*D30</f>
@@ -2836,10 +2838,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D55" s="7" t="n">
         <f aca="false">D$16*D30</f>

</xml_diff>